<commit_message>
Updated plotting for VET project
</commit_message>
<xml_diff>
--- a/projects/va_emerging_tech/data/monte_carlo_inputs.xlsx
+++ b/projects/va_emerging_tech/data/monte_carlo_inputs.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D3AF213-CE25-4E1D-A078-A399BDD32587}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E12A3F78-2F6B-4F43-A2A2-621E80568F33}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="656" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30435" yWindow="2655" windowWidth="23235" windowHeight="10440" tabRatio="656" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="example" sheetId="9" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="78">
   <si>
     <t>Ref.</t>
   </si>
@@ -249,6 +249,12 @@
   </si>
   <si>
     <t>[%/year]</t>
+  </si>
+  <si>
+    <t>CostInvest</t>
+  </si>
+  <si>
+    <t>[M$/GW]</t>
   </si>
 </sst>
 </file>
@@ -281,7 +287,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -291,6 +297,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -307,7 +319,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -325,6 +337,7 @@
     </xf>
     <xf numFmtId="11" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -607,8 +620,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H5" sqref="A1:H5"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1509,10 +1522,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B2DE492-BD1A-44A2-AB64-20C476A17F08}">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1521,7 +1534,7 @@
     <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.6640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1661,6 +1674,118 @@
         <v>0</v>
       </c>
     </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>69</v>
+      </c>
+      <c r="B6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C6" t="s">
+        <v>71</v>
+      </c>
+      <c r="D6" t="s">
+        <v>77</v>
+      </c>
+      <c r="E6">
+        <v>1884</v>
+      </c>
+      <c r="F6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" s="13">
+        <f>E6*0.8</f>
+        <v>1507.2</v>
+      </c>
+      <c r="H6" s="13">
+        <f>E6*1.2</f>
+        <v>2260.7999999999997</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>69</v>
+      </c>
+      <c r="B7" t="s">
+        <v>76</v>
+      </c>
+      <c r="C7" t="s">
+        <v>72</v>
+      </c>
+      <c r="D7" t="s">
+        <v>77</v>
+      </c>
+      <c r="E7">
+        <v>2474</v>
+      </c>
+      <c r="F7" t="s">
+        <v>8</v>
+      </c>
+      <c r="G7">
+        <f t="shared" ref="G7:G9" si="0">E7*0.8</f>
+        <v>1979.2</v>
+      </c>
+      <c r="H7">
+        <f t="shared" ref="H7:H9" si="1">E7*1.2</f>
+        <v>2968.7999999999997</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B8" t="s">
+        <v>76</v>
+      </c>
+      <c r="C8" t="s">
+        <v>73</v>
+      </c>
+      <c r="D8" t="s">
+        <v>77</v>
+      </c>
+      <c r="E8">
+        <v>1457</v>
+      </c>
+      <c r="F8" t="s">
+        <v>8</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="0"/>
+        <v>1165.6000000000001</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="1"/>
+        <v>1748.3999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>69</v>
+      </c>
+      <c r="B9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C9" t="s">
+        <v>70</v>
+      </c>
+      <c r="D9" t="s">
+        <v>77</v>
+      </c>
+      <c r="E9" s="5">
+        <v>6874</v>
+      </c>
+      <c r="F9" t="s">
+        <v>8</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="0"/>
+        <v>5499.2000000000007</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="1"/>
+        <v>8248.7999999999993</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Revising Monte Carlo inputs with alternative distributions and analysis of ATB data
</commit_message>
<xml_diff>
--- a/projects/va_emerging_tech/data/monte_carlo_inputs.xlsx
+++ b/projects/va_emerging_tech/data/monte_carlo_inputs.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E12A3F78-2F6B-4F43-A2A2-621E80568F33}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7905B74E-BE24-412D-8B92-080FEDA9818B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30435" yWindow="2655" windowWidth="23235" windowHeight="10440" tabRatio="656" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="656" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="example" sheetId="9" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="99">
   <si>
     <t>Ref.</t>
   </si>
@@ -255,6 +255,69 @@
   </si>
   <si>
     <t>[M$/GW]</t>
+  </si>
+  <si>
+    <t>EC_PUMP</t>
+  </si>
+  <si>
+    <t>EC_BATT</t>
+  </si>
+  <si>
+    <t>EC_BIO</t>
+  </si>
+  <si>
+    <t>EC_COAL</t>
+  </si>
+  <si>
+    <t>EC_OIL_CC</t>
+  </si>
+  <si>
+    <t>EC_NG_CC</t>
+  </si>
+  <si>
+    <t>EC_NG_OC</t>
+  </si>
+  <si>
+    <t>EC_SOLPV</t>
+  </si>
+  <si>
+    <t>EC_WIND</t>
+  </si>
+  <si>
+    <t>ED_BATT</t>
+  </si>
+  <si>
+    <t>ED_SOLPV</t>
+  </si>
+  <si>
+    <t>EF_WIND</t>
+  </si>
+  <si>
+    <t>20% range</t>
+  </si>
+  <si>
+    <t>assm.</t>
+  </si>
+  <si>
+    <t>ATB</t>
+  </si>
+  <si>
+    <t>CostFixedIncr</t>
+  </si>
+  <si>
+    <t>EX_SOLPV</t>
+  </si>
+  <si>
+    <t>EX_WIND</t>
+  </si>
+  <si>
+    <t>CostVariable</t>
+  </si>
+  <si>
+    <t>CostFixed</t>
+  </si>
+  <si>
+    <t>Fuel cost uncertainty?</t>
   </si>
 </sst>
 </file>
@@ -287,7 +350,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -306,6 +369,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -319,7 +394,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -338,6 +413,9 @@
     <xf numFmtId="11" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1522,16 +1600,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B2DE492-BD1A-44A2-AB64-20C476A17F08}">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39:A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.21875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.6640625" bestFit="1" customWidth="1"/>
@@ -1575,25 +1653,31 @@
         <v>69</v>
       </c>
       <c r="B2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D2" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="E2">
-        <v>-3.15</v>
+        <v>2474</v>
       </c>
       <c r="F2" t="s">
         <v>8</v>
       </c>
       <c r="G2">
-        <v>-5</v>
+        <f t="shared" ref="G2:G4" si="0">E2*0.8</f>
+        <v>1979.2</v>
       </c>
       <c r="H2">
-        <v>0</v>
+        <f t="shared" ref="H2:H4" si="1">E2*1.2</f>
+        <v>2968.7999999999997</v>
+      </c>
+      <c r="I2" s="2"/>
+      <c r="J2" s="16" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -1601,25 +1685,31 @@
         <v>69</v>
       </c>
       <c r="B3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D3" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="E3">
-        <v>-0.89</v>
+        <v>1457</v>
       </c>
       <c r="F3" t="s">
         <v>8</v>
       </c>
       <c r="G3">
-        <v>-5</v>
+        <f t="shared" si="0"/>
+        <v>1165.6000000000001</v>
       </c>
       <c r="H3">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>1748.3999999999999</v>
+      </c>
+      <c r="I3" s="2"/>
+      <c r="J3" s="16" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
@@ -1627,164 +1717,1011 @@
         <v>69</v>
       </c>
       <c r="B4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D4" t="s">
+        <v>77</v>
+      </c>
+      <c r="E4" s="5">
+        <v>6874</v>
+      </c>
+      <c r="F4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="0"/>
+        <v>5499.2000000000007</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="1"/>
+        <v>8248.7999999999993</v>
+      </c>
+      <c r="I4" s="2"/>
+      <c r="J4" s="16" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B5" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="C4" t="s">
-        <v>73</v>
-      </c>
-      <c r="D4" t="s">
-        <v>75</v>
-      </c>
-      <c r="E4">
-        <v>-1</v>
-      </c>
-      <c r="F4" t="s">
-        <v>8</v>
-      </c>
-      <c r="G4">
-        <v>-5</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>69</v>
-      </c>
-      <c r="B5" t="s">
-        <v>74</v>
-      </c>
       <c r="C5" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="D5" t="s">
         <v>75</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5">
+        <v>-1</v>
+      </c>
+      <c r="F5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="13">
+        <v>-2</v>
+      </c>
+      <c r="H5" s="13">
+        <v>0</v>
+      </c>
+      <c r="J5" s="16" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C6" t="s">
+        <v>79</v>
+      </c>
+      <c r="D6" t="s">
+        <v>75</v>
+      </c>
+      <c r="E6">
+        <v>-1.97</v>
+      </c>
+      <c r="F6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6">
+        <v>-4.2699999999999996</v>
+      </c>
+      <c r="H6">
+        <v>-0.61</v>
+      </c>
+      <c r="J6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C7" t="s">
+        <v>80</v>
+      </c>
+      <c r="D7" t="s">
+        <v>75</v>
+      </c>
+      <c r="E7">
+        <v>-0.53</v>
+      </c>
+      <c r="F7" t="s">
+        <v>8</v>
+      </c>
+      <c r="G7" s="13">
+        <v>-1</v>
+      </c>
+      <c r="H7" s="13">
+        <v>0</v>
+      </c>
+      <c r="J7" s="16" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C8" t="s">
+        <v>81</v>
+      </c>
+      <c r="D8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E8">
+        <v>-0.63</v>
+      </c>
+      <c r="F8" t="s">
+        <v>8</v>
+      </c>
+      <c r="G8" s="13">
+        <v>-1</v>
+      </c>
+      <c r="H8" s="13">
+        <v>0</v>
+      </c>
+      <c r="J8" s="16" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D9" t="s">
+        <v>75</v>
+      </c>
+      <c r="E9">
+        <v>-0.4</v>
+      </c>
+      <c r="F9" t="s">
+        <v>8</v>
+      </c>
+      <c r="G9" s="13">
+        <v>-1</v>
+      </c>
+      <c r="H9" s="13">
+        <v>0</v>
+      </c>
+      <c r="J9" s="16" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C10" t="s">
+        <v>83</v>
+      </c>
+      <c r="D10" t="s">
+        <v>75</v>
+      </c>
+      <c r="E10">
+        <v>-0.4</v>
+      </c>
+      <c r="F10" t="s">
+        <v>8</v>
+      </c>
+      <c r="G10" s="13">
+        <v>-1</v>
+      </c>
+      <c r="H10" s="13">
+        <v>0</v>
+      </c>
+      <c r="J10" s="16" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C11" t="s">
+        <v>84</v>
+      </c>
+      <c r="D11" t="s">
+        <v>75</v>
+      </c>
+      <c r="E11">
+        <v>-0.41</v>
+      </c>
+      <c r="F11" t="s">
+        <v>8</v>
+      </c>
+      <c r="G11" s="13">
+        <v>-1</v>
+      </c>
+      <c r="H11" s="13">
+        <v>0</v>
+      </c>
+      <c r="J11" s="16" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C12" t="s">
+        <v>85</v>
+      </c>
+      <c r="D12" t="s">
+        <v>75</v>
+      </c>
+      <c r="E12">
+        <v>-1.86</v>
+      </c>
+      <c r="F12" t="s">
+        <v>8</v>
+      </c>
+      <c r="G12">
+        <v>-3</v>
+      </c>
+      <c r="H12">
+        <v>-1.08</v>
+      </c>
+      <c r="J12" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C13" t="s">
+        <v>86</v>
+      </c>
+      <c r="D13" t="s">
+        <v>75</v>
+      </c>
+      <c r="E13">
+        <v>-1.7</v>
+      </c>
+      <c r="F13" t="s">
+        <v>8</v>
+      </c>
+      <c r="G13">
+        <v>-2.88</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="J13" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="E14" s="15">
+        <v>-1.97</v>
+      </c>
+      <c r="F14" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="G14" s="15">
+        <v>-4.2699999999999996</v>
+      </c>
+      <c r="H14" s="15">
+        <v>-0.61</v>
+      </c>
+      <c r="I14" s="14"/>
+      <c r="J14" s="14"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="E15" s="14">
+        <v>-2.23</v>
+      </c>
+      <c r="F15" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="G15" s="14">
+        <v>-3.45</v>
+      </c>
+      <c r="H15" s="14">
+        <v>-1.17</v>
+      </c>
+      <c r="I15" s="14"/>
+      <c r="J15" s="14"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="D16" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="E16" s="14">
+        <v>-2.14</v>
+      </c>
+      <c r="F16" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="G16" s="14">
+        <v>-3.42</v>
+      </c>
+      <c r="H16" s="14">
+        <v>0</v>
+      </c>
+      <c r="I16" s="14"/>
+      <c r="J16" s="14"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A17" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C17" t="s">
+        <v>71</v>
+      </c>
+      <c r="D17" t="s">
+        <v>75</v>
+      </c>
+      <c r="E17">
+        <v>-3.15</v>
+      </c>
+      <c r="F17" t="s">
+        <v>8</v>
+      </c>
+      <c r="G17">
+        <v>-4.5599999999999996</v>
+      </c>
+      <c r="H17">
+        <v>-2.06</v>
+      </c>
+      <c r="J17" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A18" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C18" t="s">
+        <v>72</v>
+      </c>
+      <c r="D18" t="s">
+        <v>75</v>
+      </c>
+      <c r="E18">
+        <v>-0.89</v>
+      </c>
+      <c r="F18" t="s">
+        <v>8</v>
+      </c>
+      <c r="G18" s="13">
+        <v>-5</v>
+      </c>
+      <c r="H18" s="13">
+        <v>0</v>
+      </c>
+      <c r="J18" s="16" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A19" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C19" t="s">
+        <v>73</v>
+      </c>
+      <c r="D19" t="s">
+        <v>75</v>
+      </c>
+      <c r="E19">
+        <v>-1</v>
+      </c>
+      <c r="F19" t="s">
+        <v>8</v>
+      </c>
+      <c r="G19" s="13">
+        <v>-5</v>
+      </c>
+      <c r="H19" s="13">
+        <v>0</v>
+      </c>
+      <c r="J19" s="16" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A20" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C20" t="s">
+        <v>70</v>
+      </c>
+      <c r="D20" t="s">
+        <v>75</v>
+      </c>
+      <c r="E20" s="5">
         <v>-0.81</v>
       </c>
-      <c r="F5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G5">
+      <c r="F20" t="s">
+        <v>8</v>
+      </c>
+      <c r="G20" s="13">
         <v>-5</v>
       </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>69</v>
-      </c>
-      <c r="B6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="H20" s="13">
+        <v>0</v>
+      </c>
+      <c r="J20" s="16" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>69</v>
+      </c>
+      <c r="B21" t="s">
+        <v>97</v>
+      </c>
+      <c r="C21" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="F21" t="s">
+        <v>8</v>
+      </c>
+      <c r="G21">
+        <f t="shared" ref="G21:G23" si="2">E21*0.8</f>
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <f t="shared" ref="H21:H23" si="3">E21*1.2</f>
+        <v>0</v>
+      </c>
+      <c r="J21" s="16" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>69</v>
+      </c>
+      <c r="B22" t="s">
+        <v>97</v>
+      </c>
+      <c r="C22" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="D22" s="13"/>
+      <c r="E22" s="13"/>
+      <c r="F22" t="s">
+        <v>8</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J22" s="16" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>69</v>
+      </c>
+      <c r="B23" t="s">
+        <v>97</v>
+      </c>
+      <c r="C23" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+      <c r="F23" t="s">
+        <v>8</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J23" s="16" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A24" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="C24" t="s">
+        <v>94</v>
+      </c>
+      <c r="D24" t="s">
+        <v>75</v>
+      </c>
+      <c r="E24">
+        <v>-1.86</v>
+      </c>
+      <c r="F24" t="s">
+        <v>8</v>
+      </c>
+      <c r="G24">
+        <v>-3</v>
+      </c>
+      <c r="H24">
+        <v>-1.08</v>
+      </c>
+      <c r="J24" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A25" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="C25" t="s">
+        <v>95</v>
+      </c>
+      <c r="D25" t="s">
+        <v>75</v>
+      </c>
+      <c r="E25">
+        <v>-1.88</v>
+      </c>
+      <c r="F25" t="s">
+        <v>8</v>
+      </c>
+      <c r="G25">
+        <v>-3.25</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
+      <c r="J25" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A26" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="C26" t="s">
+        <v>79</v>
+      </c>
+      <c r="D26" t="s">
+        <v>75</v>
+      </c>
+      <c r="E26">
+        <v>-1.97</v>
+      </c>
+      <c r="F26" t="s">
+        <v>8</v>
+      </c>
+      <c r="G26">
+        <v>-4.2699999999999996</v>
+      </c>
+      <c r="H26">
+        <v>-0.61</v>
+      </c>
+      <c r="J26" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A27" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="C27" t="s">
+        <v>85</v>
+      </c>
+      <c r="D27" t="s">
+        <v>75</v>
+      </c>
+      <c r="E27">
+        <v>-1.86</v>
+      </c>
+      <c r="F27" t="s">
+        <v>8</v>
+      </c>
+      <c r="G27">
+        <v>-3</v>
+      </c>
+      <c r="H27">
+        <v>-1.08</v>
+      </c>
+      <c r="J27" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A28" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="C28" t="s">
+        <v>86</v>
+      </c>
+      <c r="D28" t="s">
+        <v>75</v>
+      </c>
+      <c r="E28">
+        <v>-1.88</v>
+      </c>
+      <c r="F28" t="s">
+        <v>8</v>
+      </c>
+      <c r="G28">
+        <v>-3.25</v>
+      </c>
+      <c r="H28">
+        <v>0</v>
+      </c>
+      <c r="J28" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A29" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="C29" t="s">
+        <v>87</v>
+      </c>
+      <c r="D29" t="s">
+        <v>75</v>
+      </c>
+      <c r="E29">
+        <v>-1.97</v>
+      </c>
+      <c r="F29" t="s">
+        <v>8</v>
+      </c>
+      <c r="G29">
+        <v>-4.2699999999999996</v>
+      </c>
+      <c r="H29">
+        <v>-0.61</v>
+      </c>
+      <c r="J29" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A30" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="C30" t="s">
+        <v>88</v>
+      </c>
+      <c r="D30" t="s">
+        <v>75</v>
+      </c>
+      <c r="E30">
+        <v>-2.23</v>
+      </c>
+      <c r="F30" t="s">
+        <v>8</v>
+      </c>
+      <c r="G30">
+        <v>-3.45</v>
+      </c>
+      <c r="H30">
+        <v>-1.17</v>
+      </c>
+      <c r="J30" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A31" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="C31" t="s">
+        <v>89</v>
+      </c>
+      <c r="D31" t="s">
+        <v>75</v>
+      </c>
+      <c r="E31">
+        <v>-2.0499999999999998</v>
+      </c>
+      <c r="F31" t="s">
+        <v>8</v>
+      </c>
+      <c r="G31">
+        <v>-3.39</v>
+      </c>
+      <c r="H31">
+        <v>0</v>
+      </c>
+      <c r="J31" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A32" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B32" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="C32" t="s">
         <v>71</v>
       </c>
-      <c r="D6" t="s">
-        <v>77</v>
-      </c>
-      <c r="E6">
-        <v>1884</v>
-      </c>
-      <c r="F6" t="s">
-        <v>8</v>
-      </c>
-      <c r="G6" s="13">
-        <f>E6*0.8</f>
-        <v>1507.2</v>
-      </c>
-      <c r="H6" s="13">
-        <f>E6*1.2</f>
-        <v>2260.7999999999997</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>69</v>
-      </c>
-      <c r="B7" t="s">
-        <v>76</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="D32" t="s">
+        <v>75</v>
+      </c>
+      <c r="E32">
+        <v>-3.15</v>
+      </c>
+      <c r="F32" t="s">
+        <v>8</v>
+      </c>
+      <c r="G32">
+        <v>-4.5599999999999996</v>
+      </c>
+      <c r="H32">
+        <v>-2.06</v>
+      </c>
+      <c r="J32" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A33" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="C33" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="D7" t="s">
-        <v>77</v>
-      </c>
-      <c r="E7">
-        <v>2474</v>
-      </c>
-      <c r="F7" t="s">
-        <v>8</v>
-      </c>
-      <c r="G7">
-        <f t="shared" ref="G7:G9" si="0">E7*0.8</f>
-        <v>1979.2</v>
-      </c>
-      <c r="H7">
-        <f t="shared" ref="H7:H9" si="1">E7*1.2</f>
-        <v>2968.7999999999997</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>69</v>
-      </c>
-      <c r="B8" t="s">
-        <v>76</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="D33" t="s">
+        <v>75</v>
+      </c>
+      <c r="F33" t="s">
+        <v>8</v>
+      </c>
+      <c r="G33">
+        <v>-5</v>
+      </c>
+      <c r="H33">
+        <v>0</v>
+      </c>
+      <c r="J33" s="16" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A34" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="C34" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="D8" t="s">
-        <v>77</v>
-      </c>
-      <c r="E8">
-        <v>1457</v>
-      </c>
-      <c r="F8" t="s">
-        <v>8</v>
-      </c>
-      <c r="G8">
-        <f t="shared" si="0"/>
-        <v>1165.6000000000001</v>
-      </c>
-      <c r="H8">
-        <f t="shared" si="1"/>
-        <v>1748.3999999999999</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>69</v>
-      </c>
-      <c r="B9" t="s">
-        <v>76</v>
-      </c>
-      <c r="C9" t="s">
+      <c r="D34" t="s">
+        <v>75</v>
+      </c>
+      <c r="F34" t="s">
+        <v>8</v>
+      </c>
+      <c r="G34">
+        <v>-5</v>
+      </c>
+      <c r="H34">
+        <v>0</v>
+      </c>
+      <c r="J34" s="16" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A35" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="C35" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="D9" t="s">
-        <v>77</v>
-      </c>
-      <c r="E9" s="5">
-        <v>6874</v>
-      </c>
-      <c r="F9" t="s">
-        <v>8</v>
-      </c>
-      <c r="G9">
-        <f t="shared" si="0"/>
-        <v>5499.2000000000007</v>
-      </c>
-      <c r="H9">
-        <f t="shared" si="1"/>
-        <v>8248.7999999999993</v>
-      </c>
+      <c r="D35" t="s">
+        <v>75</v>
+      </c>
+      <c r="F35" t="s">
+        <v>8</v>
+      </c>
+      <c r="G35">
+        <v>-5</v>
+      </c>
+      <c r="H35">
+        <v>0</v>
+      </c>
+      <c r="J35" s="16" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>69</v>
+      </c>
+      <c r="B36" t="s">
+        <v>96</v>
+      </c>
+      <c r="C36" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="D36" s="13"/>
+      <c r="E36" s="13"/>
+      <c r="F36" t="s">
+        <v>8</v>
+      </c>
+      <c r="G36">
+        <f t="shared" ref="G36:G38" si="4">E36*0.8</f>
+        <v>0</v>
+      </c>
+      <c r="H36">
+        <f t="shared" ref="H36:H38" si="5">E36*1.2</f>
+        <v>0</v>
+      </c>
+      <c r="J36" s="16" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>69</v>
+      </c>
+      <c r="B37" t="s">
+        <v>96</v>
+      </c>
+      <c r="C37" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="D37" s="13"/>
+      <c r="E37" s="13"/>
+      <c r="F37" t="s">
+        <v>8</v>
+      </c>
+      <c r="G37">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="H37">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J37" s="16" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>69</v>
+      </c>
+      <c r="B38" t="s">
+        <v>96</v>
+      </c>
+      <c r="C38" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="D38" s="13"/>
+      <c r="E38" s="13"/>
+      <c r="F38" t="s">
+        <v>8</v>
+      </c>
+      <c r="G38">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="H38">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J38" s="16" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A39" s="13" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A40" s="13"/>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A41" s="13"/>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A42" s="13"/>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A43" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>